<commit_message>
Excel Test Driver changes
</commit_message>
<xml_diff>
--- a/model/processed_outputIDHJ-EGNY.xlsx
+++ b/model/processed_outputIDHJ-EGNY.xlsx
@@ -2552,7 +2552,7 @@
         <v>44601.0</v>
       </c>
       <c r="B2" t="n" s="70">
-        <v>44601.0</v>
+        <v>44600.0</v>
       </c>
       <c r="C2" t="n" s="69">
         <v>44595.0</v>
@@ -2772,7 +2772,7 @@
         <v>2.0220131E7</v>
       </c>
       <c r="C2" t="n" s="68">
-        <v>44592.020833333336</v>
+        <v>44592.0</v>
       </c>
       <c r="D2" t="s">
         <v>77</v>
@@ -2855,7 +2855,7 @@
       </c>
       <c r="F3" s="9" t="n">
         <f>i_InstrumentAttribute!C2</f>
-        <v>44592.020833333336</v>
+        <v>44592.0</v>
       </c>
       <c r="H3" s="60" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
model execution changes, aggregation code refactoring
</commit_message>
<xml_diff>
--- a/model/processed_outputIDHJ-EGNY.xlsx
+++ b/model/processed_outputIDHJ-EGNY.xlsx
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="97">
   <si>
     <t>Date</t>
   </si>
@@ -285,28 +285,58 @@
     <t>REMIT</t>
   </si>
   <si>
-    <t>1.0</t>
+    <t>20220209</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>-350.0</t>
+  </si>
+  <si>
+    <t>-275.0</t>
+  </si>
+  <si>
+    <t>-200.0</t>
   </si>
   <si>
     <t>REMIT REVERSAL</t>
   </si>
   <si>
+    <t>200.0</t>
+  </si>
+  <si>
+    <t>99441.5918</t>
+  </si>
+  <si>
+    <t>202202</t>
+  </si>
+  <si>
+    <t>100000.0000</t>
+  </si>
+  <si>
     <t>UNPAID PRINCIPAL BALANCE</t>
   </si>
   <si>
+    <t>558.4082</t>
+  </si>
+  <si>
+    <t>55.2454</t>
+  </si>
+  <si>
+    <t>155.5556</t>
+  </si>
+  <si>
     <t>ACCRUED INTEREST RECEIVABLE</t>
   </si>
   <si>
+    <t>100.3102</t>
+  </si>
+  <si>
     <t>ACTUAL_360</t>
   </si>
   <si>
-    <t>2023-01-31</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>2022-01-31</t>
+    <t>20220131</t>
   </si>
 </sst>
 </file>
@@ -318,7 +348,7 @@
     <numFmt numFmtId="165" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="166" formatCode="#,##0.0000_);[Red]\(#,##0.0000\)"/>
     <numFmt numFmtId="167" formatCode="0.0000_);[Red]\(0.0000\)"/>
-    <numFmt numFmtId="168" formatCode="MM/dd/yyyy"/>
+    <numFmt numFmtId="168" formatCode="M/dd/yyyy"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -500,7 +530,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
@@ -578,6 +608,8 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -2548,13 +2580,13 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n" s="71">
+      <c r="A2" t="n" s="73">
         <v>44601.0</v>
       </c>
-      <c r="B2" t="n" s="70">
+      <c r="B2" t="n" s="72">
         <v>44600.0</v>
       </c>
-      <c r="C2" t="n" s="69">
+      <c r="C2" t="n" s="71">
         <v>44595.0</v>
       </c>
     </row>
@@ -2603,104 +2635,104 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="B2" t="n">
-        <v>2.0220209E7</v>
+      <c r="B2" t="s" s="2">
+        <v>79</v>
       </c>
       <c r="C2" t="n" s="63">
         <v>44601.0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" t="n">
-        <v>100.0</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="E2" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F2" t="s" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="B3" t="n">
-        <v>2.0220209E7</v>
+      <c r="B3" t="s" s="2">
+        <v>79</v>
       </c>
       <c r="C3" t="n" s="64">
         <v>44598.0</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="E3" t="s">
-        <v>79</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-350.0</v>
-      </c>
-    </row>
-    <row r="4">
+      <c r="E3" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F3" t="s" s="2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="B4" t="n">
-        <v>2.0220209E7</v>
+      <c r="B4" t="s" s="2">
+        <v>79</v>
       </c>
       <c r="C4" t="n" s="65">
         <v>44597.0</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-275.0</v>
-      </c>
-    </row>
-    <row r="5">
+      <c r="E4" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F4" t="s" s="2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s" s="2">
         <v>78</v>
       </c>
-      <c r="B5" t="n">
-        <v>2.0220209E7</v>
+      <c r="B5" t="s" s="2">
+        <v>79</v>
       </c>
       <c r="C5" t="n" s="66">
         <v>44595.0</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F5" t="s" s="2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s" s="2">
         <v>79</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-200.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s" s="2">
-        <v>80</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2.0220209E7</v>
       </c>
       <c r="C6" t="n" s="67">
         <v>44595.0</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="E6" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" t="n">
-        <v>200.0</v>
+      <c r="E6" t="n" s="2">
+        <v>1.0</v>
+      </c>
+      <c r="F6" t="s" s="2">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -2767,31 +2799,35 @@
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
     </row>
-    <row r="2">
-      <c r="B2" t="n" s="2">
-        <v>2.0220131E7</v>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>96</v>
       </c>
       <c r="C2" t="n" s="68">
         <v>44592.0</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" t="s">
-        <v>85</v>
+      <c r="E2" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>10.0</v>
       </c>
       <c r="G2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" t="s">
-        <v>84</v>
-      </c>
-      <c r="I2" t="s">
-        <v>86</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="H2" t="n" s="69">
+        <v>44957.0</v>
+      </c>
+      <c r="I2" t="n" s="70">
+        <v>44592.0</v>
+      </c>
+      <c r="J2" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -2954,11 +2990,11 @@
       <c r="A8" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="45" t="n">
+      <c r="B8" s="45" t="str">
         <f>IF(i_Metric!G2="","",i_Metric!G2)</f>
-        <v>100000.0</v>
-      </c>
-      <c r="C8" s="45" t="n">
+        <v>100000.0000</v>
+      </c>
+      <c r="C8" s="45" t="str">
         <f>IF(i_Metric!G3="","",i_Metric!G3)</f>
         <v>155.5556</v>
       </c>
@@ -3035,7 +3071,7 @@
         <f t="shared" ref="C12:F12" si="0">C13</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D12" s="17" t="str">
+      <c r="D12" s="17" t="n">
         <f t="shared" si="0"/>
         <v>1.0</v>
       </c>
@@ -3043,7 +3079,7 @@
         <f t="shared" si="0"/>
         <v>ACTUAL_360</v>
       </c>
-      <c r="F12" s="4" t="str">
+      <c r="F12" s="4" t="n">
         <f t="shared" si="0"/>
         <v>10.0</v>
       </c>
@@ -3092,7 +3128,7 @@
         <f>C14</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D13" s="17" t="str">
+      <c r="D13" s="17" t="n">
         <f>D14</f>
         <v>1.0</v>
       </c>
@@ -3100,7 +3136,7 @@
         <f>E14</f>
         <v>ACTUAL_360</v>
       </c>
-      <c r="F13" s="4" t="str">
+      <c r="F13" s="4" t="n">
         <f>F14</f>
         <v>10.0</v>
       </c>
@@ -3146,7 +3182,7 @@
         <f t="shared" ref="C14:F15" si="6">C15</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D14" s="17" t="str">
+      <c r="D14" s="17" t="n">
         <f t="shared" si="6"/>
         <v>1.0</v>
       </c>
@@ -3154,7 +3190,7 @@
         <f t="shared" si="6"/>
         <v>ACTUAL_360</v>
       </c>
-      <c r="F14" s="4" t="str">
+      <c r="F14" s="4" t="n">
         <f t="shared" si="6"/>
         <v>10.0</v>
       </c>
@@ -3200,7 +3236,7 @@
         <f t="shared" si="6"/>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D15" s="17" t="str">
+      <c r="D15" s="17" t="n">
         <f t="shared" si="6"/>
         <v>1.0</v>
       </c>
@@ -3208,7 +3244,7 @@
         <f t="shared" si="6"/>
         <v>ACTUAL_360</v>
       </c>
-      <c r="F15" s="4" t="str">
+      <c r="F15" s="4" t="n">
         <f t="shared" si="6"/>
         <v>10.0</v>
       </c>
@@ -3255,7 +3291,7 @@
         <f>IF(i_InstrumentAttribute!D2="","",i_InstrumentAttribute!D2)</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D16" s="17" t="str">
+      <c r="D16" s="17" t="n">
         <f>IF(i_InstrumentAttribute!E2="","",i_InstrumentAttribute!E2)</f>
         <v>1.0</v>
       </c>
@@ -3263,7 +3299,7 @@
         <f>IF(i_InstrumentAttribute!G2="","",i_InstrumentAttribute!G2)</f>
         <v>ACTUAL_360</v>
       </c>
-      <c r="F16" s="4" t="str">
+      <c r="F16" s="4" t="n">
         <f>IF(i_InstrumentAttribute!F2="","",i_InstrumentAttribute!F2)</f>
         <v>10.0</v>
       </c>
@@ -3353,9 +3389,9 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="n">
+      <c r="A21" s="9" t="str">
         <f>IF(i_Transaction!B2="","",i_Transaction!B2)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B21" s="9" t="n">
         <f>IF(i_Transaction!C2="","",i_Transaction!C2)</f>
@@ -3365,7 +3401,7 @@
         <f>IF(i_Transaction!D2="","",i_Transaction!D2)</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D21" s="17" t="str">
+      <c r="D21" s="17" t="n">
         <f>IF(i_Transaction!E2="","",i_Transaction!E2)</f>
         <v>1.0</v>
       </c>
@@ -3391,9 +3427,9 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="n">
+      <c r="A22" s="9" t="str">
         <f>IF(i_Transaction!B3="","",i_Transaction!B3)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B22" s="9" t="n">
         <f>IF(i_Transaction!C3="","",i_Transaction!C3)</f>
@@ -3403,7 +3439,7 @@
         <f>IF(i_Transaction!D3="","",i_Transaction!D3)</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D22" s="17" t="str">
+      <c r="D22" s="17" t="n">
         <f>IF(i_Transaction!E3="","",i_Transaction!E3)</f>
         <v>1.0</v>
       </c>
@@ -3425,13 +3461,13 @@
       </c>
       <c r="I22" s="45" t="str">
         <f>IF(i_Transaction!F3="","",IF(AND(i_Transaction!F3&lt;=0,F22&lt;&gt;0),"Reversal","New"))</f>
-        <v>Reversal</v>
+        <v>New</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="n">
+      <c r="A23" s="9" t="str">
         <f>IF(i_Transaction!B4="","",i_Transaction!B4)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B23" s="9" t="n">
         <f>IF(i_Transaction!C4="","",i_Transaction!C4)</f>
@@ -3441,7 +3477,7 @@
         <f>IF(i_Transaction!D4="","",i_Transaction!D4)</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D23" s="17" t="str">
+      <c r="D23" s="17" t="n">
         <f>IF(i_Transaction!E4="","",i_Transaction!E4)</f>
         <v>1.0</v>
       </c>
@@ -3463,13 +3499,13 @@
       </c>
       <c r="I23" s="45" t="str">
         <f>IF(i_Transaction!F4="","",IF(AND(i_Transaction!F4&lt;=0,F23&lt;&gt;0),"Reversal","New"))</f>
-        <v>Reversal</v>
+        <v>New</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="n">
+      <c r="A24" s="9" t="str">
         <f>IF(i_Transaction!B5="","",i_Transaction!B5)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B24" s="9" t="n">
         <f>IF(i_Transaction!C5="","",i_Transaction!C5)</f>
@@ -3479,11 +3515,11 @@
         <f>IF(i_Transaction!D5="","",i_Transaction!D5)</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="D24" s="17" t="str">
+      <c r="D24" s="17" t="n">
         <f>IF(i_Transaction!E5="","",i_Transaction!E5)</f>
         <v>1.0</v>
       </c>
-      <c r="E24" s="46" t="n">
+      <c r="E24" s="46" t="str">
         <f>C8</f>
         <v>155.5556</v>
       </c>
@@ -3582,7 +3618,7 @@
         <f>IFERROR(IF(M13=0,"",M13),0)</f>
         <v>83.0346</v>
       </c>
-      <c r="F30" s="4" t="str">
+      <c r="F30" s="4" t="n">
         <f>IF(A30="","",D13)</f>
         <v>1.0</v>
       </c>
@@ -3608,7 +3644,7 @@
         <f>IFERROR(IF(M14=0,"",M14),0)</f>
         <v>27.7677</v>
       </c>
-      <c r="F31" s="4" t="str">
+      <c r="F31" s="4" t="n">
         <f>IF(A31="","",D14)</f>
         <v>1.0</v>
       </c>
@@ -3634,7 +3670,7 @@
         <f>IFERROR(IF(M15=0,"",M15),0)</f>
         <v>55.5556</v>
       </c>
-      <c r="F32" s="4" t="str">
+      <c r="F32" s="4" t="n">
         <f>IF(A32="","",D15)</f>
         <v>1.0</v>
       </c>
@@ -3660,15 +3696,15 @@
         <f>IFERROR(IF(M16=0,"",M16),0)</f>
         <v>27.7778</v>
       </c>
-      <c r="F33" s="4" t="str">
+      <c r="F33" s="4" t="n">
         <f>IF(A33="","",D16)</f>
         <v>1.0</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="n">
+      <c r="A34" s="9" t="str">
         <f>IF(E34="","",A21)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B34" s="9" t="n">
         <f>IF(A34="","",B21)</f>
@@ -3686,15 +3722,15 @@
         <f>IFERROR(IF(G21=0,"",-G21),0)</f>
         <v>-83.0346</v>
       </c>
-      <c r="F34" s="4" t="str">
+      <c r="F34" s="4" t="n">
         <f>IF(A34="","",D21)</f>
         <v>1.0</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="9" t="n">
+      <c r="A35" s="9" t="str">
         <f>IF(E35="","",A22)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B35" s="9" t="n">
         <f>IF(A35="","",B22)</f>
@@ -3712,15 +3748,15 @@
         <f>IFERROR(IF(G22=0,"",-G22),0)</f>
         <v>-27.7677</v>
       </c>
-      <c r="F35" s="4" t="str">
+      <c r="F35" s="4" t="n">
         <f>IF(A35="","",D22)</f>
         <v>1.0</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="n">
+      <c r="A36" s="9" t="str">
         <f>IF(E36="","",A23)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B36" s="9" t="n">
         <f>IF(A36="","",B23)</f>
@@ -3738,7 +3774,7 @@
         <f>IFERROR(IF(G23=0,"",-G23),0)</f>
         <v>-238.889</v>
       </c>
-      <c r="F36" s="4" t="str">
+      <c r="F36" s="4" t="n">
         <f>IF(A36="","",D23)</f>
         <v>1.0</v>
       </c>
@@ -3770,9 +3806,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="9" t="n">
+      <c r="A38" s="9" t="str">
         <f>IF(E38="","",A21)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B38" s="9" t="n">
         <f>IF(A38="","",B21)</f>
@@ -3790,15 +3826,15 @@
         <f>IFERROR(IF(H21=0,"",-H21),0)</f>
         <v>-16.9654</v>
       </c>
-      <c r="F38" s="4" t="str">
+      <c r="F38" s="4" t="n">
         <f>IF(A38="","",D21)</f>
         <v>1.0</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="9" t="n">
+      <c r="A39" s="9" t="str">
         <f>IF(E39="","",A22)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B39" s="9" t="n">
         <f>IF(A39="","",B22)</f>
@@ -3816,15 +3852,15 @@
         <f>IFERROR(IF(H22=0,"",-H22),0)</f>
         <v>-322.2323</v>
       </c>
-      <c r="F39" s="4" t="str">
+      <c r="F39" s="4" t="n">
         <f>IF(A39="","",D22)</f>
         <v>1.0</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="9" t="n">
+      <c r="A40" s="9" t="str">
         <f>IF(E40="","",A23)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="B40" s="9" t="n">
         <f>IF(A40="","",B23)</f>
@@ -3842,7 +3878,7 @@
         <f>IFERROR(IF(H23=0,"",-H23),0)</f>
         <v>-36.111</v>
       </c>
-      <c r="F40" s="4" t="str">
+      <c r="F40" s="4" t="n">
         <f>IF(A40="","",D23)</f>
         <v>1.0</v>
       </c>
@@ -3900,55 +3936,55 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="9" t="n">
+      <c r="A43" s="9" t="str">
         <f>IF(E43="","",A22)</f>
-        <v>2.0220209E7</v>
-      </c>
-      <c r="B43" s="9" t="n">
+        <v/>
+      </c>
+      <c r="B43" s="9" t="str">
         <f>IF(A43="","",B22)</f>
-        <v>44598.0</v>
+        <v/>
       </c>
       <c r="C43" s="4" t="str">
         <f>IF(A43="","",C22)</f>
-        <v>IDHJ-EGNY</v>
+        <v/>
       </c>
       <c r="D43" s="13" t="str">
         <f>IF(A43="","","Remit")</f>
-        <v>Remit</v>
-      </c>
-      <c r="E43" s="47" t="n">
+        <v/>
+      </c>
+      <c r="E43" s="47" t="str">
         <f t="shared" ref="E43:E45" si="7">IFERROR(IF(OR(F22=0,I22="New"),"",F22),0)</f>
-        <v>350.0</v>
+        <v/>
       </c>
       <c r="F43" s="4" t="str">
         <f>IF(A43="","",D22)</f>
-        <v>1.0</v>
+        <v/>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="9" t="n">
+      <c r="A44" s="9" t="str">
         <f>IF(E44="","",A23)</f>
-        <v>2.0220209E7</v>
-      </c>
-      <c r="B44" s="9" t="n">
+        <v/>
+      </c>
+      <c r="B44" s="9" t="str">
         <f>IF(A44="","",B23)</f>
-        <v>44597.0</v>
+        <v/>
       </c>
       <c r="C44" s="4" t="str">
         <f>IF(A44="","",C23)</f>
-        <v>IDHJ-EGNY</v>
+        <v/>
       </c>
       <c r="D44" s="13" t="str">
         <f>IF(A44="","","Remit")</f>
-        <v>Remit</v>
-      </c>
-      <c r="E44" s="47" t="n">
+        <v/>
+      </c>
+      <c r="E44" s="47" t="str">
         <f t="shared" si="7"/>
-        <v>275.0</v>
+        <v/>
       </c>
       <c r="F44" s="4" t="str">
         <f>IF(A44="","",D23)</f>
-        <v>1.0</v>
+        <v/>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -4021,13 +4057,13 @@
         <f>C16</f>
         <v>IDHJ-EGNY</v>
       </c>
-      <c r="C50" s="17" t="str">
+      <c r="C50" s="17" t="n">
         <f>D16</f>
         <v>1.0</v>
       </c>
-      <c r="D50" s="9" t="str">
+      <c r="D50" s="9" t="n">
         <f>IF(i_InstrumentAttribute!H2="","",i_InstrumentAttribute!H2)</f>
-        <v>2023-01-31</v>
+        <v>44957.0</v>
       </c>
       <c r="E50" s="9" t="str">
         <f>IF(A50=D50,D50,"")</f>
@@ -4097,44 +4133,46 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s" s="2">
-        <v>81</v>
-      </c>
-      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="D2" t="n">
-        <v>202202.0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>99441.5918</v>
-      </c>
-      <c r="F2" t="n">
-        <v>558.4082</v>
-      </c>
-      <c r="G2" t="n">
-        <v>100000.0</v>
-      </c>
-    </row>
-    <row r="3">
+      <c r="D2" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="E2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s" s="2">
-        <v>82</v>
-      </c>
-      <c r="C3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" t="s" s="2">
         <v>77</v>
       </c>
-      <c r="D3" t="n">
-        <v>202202.0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>55.2454</v>
-      </c>
-      <c r="F3" t="n">
-        <v>100.3102</v>
-      </c>
-      <c r="G3" t="n">
-        <v>155.5556</v>
+      <c r="D3" t="s" s="2">
+        <v>87</v>
+      </c>
+      <c r="E3" t="s">
+        <v>91</v>
+      </c>
+      <c r="F3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G3" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -4230,7 +4268,7 @@
         <f>IF(A3="","",CALC!E30)</f>
         <v>83.0346</v>
       </c>
-      <c r="F3" s="15" t="str">
+      <c r="F3" s="15" t="n">
         <f>IF(E3="","",CALC!F30)</f>
         <v>1.0</v>
       </c>
@@ -4256,7 +4294,7 @@
         <f>IF(A4="","",CALC!E31)</f>
         <v>27.7677</v>
       </c>
-      <c r="F4" s="15" t="str">
+      <c r="F4" s="15" t="n">
         <f>IF(E4="","",CALC!F31)</f>
         <v>1.0</v>
       </c>
@@ -4282,7 +4320,7 @@
         <f>IF(A5="","",CALC!E32)</f>
         <v>55.5556</v>
       </c>
-      <c r="F5" s="15" t="str">
+      <c r="F5" s="15" t="n">
         <f>IF(E5="","",CALC!F32)</f>
         <v>1.0</v>
       </c>
@@ -4308,7 +4346,7 @@
         <f>IF(A6="","",CALC!E33)</f>
         <v>27.7778</v>
       </c>
-      <c r="F6" s="15" t="str">
+      <c r="F6" s="15" t="n">
         <f>IF(E6="","",CALC!F33)</f>
         <v>1.0</v>
       </c>
@@ -4318,9 +4356,9 @@
         <f>IF(D7="","",CALC!D34)</f>
         <v>Payment - Interest</v>
       </c>
-      <c r="B7" s="8" t="n">
+      <c r="B7" s="8" t="str">
         <f>IF(CALC!A34="","",CALC!A34)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="C7" s="8" t="n">
         <f>IF(B7="","",CALC!B34)</f>
@@ -4334,7 +4372,7 @@
         <f>IF(A7="","",CALC!E34)</f>
         <v>-83.0346</v>
       </c>
-      <c r="F7" s="15" t="str">
+      <c r="F7" s="15" t="n">
         <f>IF(E7="","",CALC!F34)</f>
         <v>1.0</v>
       </c>
@@ -4344,9 +4382,9 @@
         <f>IF(D8="","",CALC!D35)</f>
         <v>Payment - Interest</v>
       </c>
-      <c r="B8" s="8" t="n">
+      <c r="B8" s="8" t="str">
         <f>IF(CALC!A35="","",CALC!A35)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="C8" s="8" t="n">
         <f>IF(B8="","",CALC!B35)</f>
@@ -4360,7 +4398,7 @@
         <f>IF(A8="","",CALC!E35)</f>
         <v>-27.7677</v>
       </c>
-      <c r="F8" s="15" t="str">
+      <c r="F8" s="15" t="n">
         <f>IF(E8="","",CALC!F35)</f>
         <v>1.0</v>
       </c>
@@ -4370,9 +4408,9 @@
         <f>IF(D9="","",CALC!D36)</f>
         <v>Payment - Interest</v>
       </c>
-      <c r="B9" s="8" t="n">
+      <c r="B9" s="8" t="str">
         <f>IF(CALC!A36="","",CALC!A36)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="C9" s="8" t="n">
         <f>IF(B9="","",CALC!B36)</f>
@@ -4386,7 +4424,7 @@
         <f>IF(A9="","",CALC!E36)</f>
         <v>-238.889</v>
       </c>
-      <c r="F9" s="15" t="str">
+      <c r="F9" s="15" t="n">
         <f>IF(E9="","",CALC!F36)</f>
         <v>1.0</v>
       </c>
@@ -4422,9 +4460,9 @@
         <f>IF(D11="","",CALC!D38)</f>
         <v>Payment - UPB</v>
       </c>
-      <c r="B11" s="8" t="n">
+      <c r="B11" s="8" t="str">
         <f>IF(CALC!A38="","",CALC!A38)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="C11" s="8" t="n">
         <f>IF(B11="","",CALC!B38)</f>
@@ -4438,7 +4476,7 @@
         <f>IF(A11="","",CALC!E38)</f>
         <v>-16.9654</v>
       </c>
-      <c r="F11" s="15" t="str">
+      <c r="F11" s="15" t="n">
         <f>IF(E11="","",CALC!F38)</f>
         <v>1.0</v>
       </c>
@@ -4448,9 +4486,9 @@
         <f>IF(D12="","",CALC!D39)</f>
         <v>Payment - UPB</v>
       </c>
-      <c r="B12" s="8" t="n">
+      <c r="B12" s="8" t="str">
         <f>IF(CALC!A39="","",CALC!A39)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="C12" s="8" t="n">
         <f>IF(B12="","",CALC!B39)</f>
@@ -4464,7 +4502,7 @@
         <f>IF(A12="","",CALC!E39)</f>
         <v>-322.2323</v>
       </c>
-      <c r="F12" s="15" t="str">
+      <c r="F12" s="15" t="n">
         <f>IF(E12="","",CALC!F39)</f>
         <v>1.0</v>
       </c>
@@ -4474,9 +4512,9 @@
         <f>IF(D13="","",CALC!D40)</f>
         <v>Payment - UPB</v>
       </c>
-      <c r="B13" s="8" t="n">
+      <c r="B13" s="8" t="str">
         <f>IF(CALC!A40="","",CALC!A40)</f>
-        <v>2.0220209E7</v>
+        <v>20220209</v>
       </c>
       <c r="C13" s="8" t="n">
         <f>IF(B13="","",CALC!B40)</f>
@@ -4490,7 +4528,7 @@
         <f>IF(A13="","",CALC!E40)</f>
         <v>-36.111</v>
       </c>
-      <c r="F13" s="15" t="str">
+      <c r="F13" s="15" t="n">
         <f>IF(E13="","",CALC!F40)</f>
         <v>1.0</v>
       </c>
@@ -4550,53 +4588,53 @@
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="str">
         <f>IF(D16="","",CALC!D43)</f>
-        <v>Remit</v>
-      </c>
-      <c r="B16" s="8" t="n">
+        <v/>
+      </c>
+      <c r="B16" s="8" t="str">
         <f>IF(CALC!A43="","",CALC!A43)</f>
-        <v>2.0220209E7</v>
-      </c>
-      <c r="C16" s="8" t="n">
+        <v/>
+      </c>
+      <c r="C16" s="8" t="str">
         <f>IF(B16="","",CALC!B43)</f>
-        <v>44598.0</v>
+        <v/>
       </c>
       <c r="D16" s="8" t="str">
         <f>IF(C16="","",CALC!C43)</f>
-        <v>IDHJ-EGNY</v>
-      </c>
-      <c r="E16" s="14" t="n">
+        <v/>
+      </c>
+      <c r="E16" s="14" t="str">
         <f>IF(A16="","",CALC!E43)</f>
-        <v>350.0</v>
+        <v/>
       </c>
       <c r="F16" s="15" t="str">
         <f>IF(E16="","",CALC!F43)</f>
-        <v>1.0</v>
+        <v/>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="str">
         <f>IF(D17="","",CALC!D44)</f>
-        <v>Remit</v>
-      </c>
-      <c r="B17" s="8" t="n">
+        <v/>
+      </c>
+      <c r="B17" s="8" t="str">
         <f>IF(CALC!A44="","",CALC!A44)</f>
-        <v>2.0220209E7</v>
-      </c>
-      <c r="C17" s="8" t="n">
+        <v/>
+      </c>
+      <c r="C17" s="8" t="str">
         <f>IF(B17="","",CALC!B44)</f>
-        <v>44597.0</v>
+        <v/>
       </c>
       <c r="D17" s="8" t="str">
         <f>IF(C17="","",CALC!C44)</f>
-        <v>IDHJ-EGNY</v>
-      </c>
-      <c r="E17" s="14" t="n">
+        <v/>
+      </c>
+      <c r="E17" s="14" t="str">
         <f>IF(A17="","",CALC!E44)</f>
-        <v>275.0</v>
+        <v/>
       </c>
       <c r="F17" s="15" t="str">
         <f>IF(E17="","",CALC!F44)</f>
-        <v>1.0</v>
+        <v/>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>